<commit_message>
Update timesheet period Juni - July
</commit_message>
<xml_diff>
--- a/7_Period_20_Jun_2024_sd_19_Jul_2024/Timesheet Danamon-Bayu Bagus Bagaswara-Juni.xlsx
+++ b/7_Period_20_Jun_2024_sd_19_Jul_2024/Timesheet Danamon-Bayu Bagus Bagaswara-Juni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\timesheet-danamon\7_Period_20_Jun_2024_sd_19_Jul_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\7_Period_20_Jun_2024_sd_19_Jul_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F52F15-AEE4-4053-AAFE-872E9DF2B30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8C1BF5-BD51-4158-9F4A-6E3E6E76918E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$AG$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$AG$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>TIME SHEET</t>
   </si>
@@ -175,16 +175,19 @@
     <t>Bayu Bagus Bagaswara</t>
   </si>
   <si>
-    <t>Diskusi alur bisnis Billing dengan User</t>
-  </si>
-  <si>
-    <t>Pengembangan fitur Billing</t>
-  </si>
-  <si>
-    <t>Diskusi dengan tim developer Billing</t>
-  </si>
-  <si>
     <t>20 Juni - 19 Juli</t>
+  </si>
+  <si>
+    <t>Support UAT Release 8 - Billing</t>
+  </si>
+  <si>
+    <t>Preparation implementation Relase 8 - Billing</t>
+  </si>
+  <si>
+    <t>Discuss with the team Release 9B - Regulatory (LKPBU &amp; LBABK)</t>
+  </si>
+  <si>
+    <t>Development Release 9B - Regulatory (LKPBU &amp; LBABK)</t>
   </si>
 </sst>
 </file>
@@ -1090,20 +1093,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EP19"/>
+  <dimension ref="A1:EP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="15.1796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="62.81640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="60.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="7.1796875" style="6" customWidth="1"/>
-    <col min="33" max="33" width="18.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.453125" style="6" customWidth="1"/>
-    <col min="35" max="35" width="14" style="6" customWidth="1"/>
+    <col min="33" max="33" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.6328125" style="6" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="11.81640625" style="6" customWidth="1"/>
     <col min="37" max="37" width="14" style="6" customWidth="1"/>
     <col min="38" max="38" width="12.54296875" style="6" customWidth="1"/>
@@ -1232,7 +1235,7 @@
       <c r="M6" s="66"/>
       <c r="N6" s="66"/>
       <c r="O6" s="70" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P6" s="71"/>
       <c r="Q6" s="71"/>
@@ -1702,24 +1705,48 @@
     <row r="11" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A11" s="36"/>
       <c r="B11" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
+        <v>28</v>
+      </c>
+      <c r="C11" s="50">
+        <v>7</v>
+      </c>
+      <c r="D11" s="50">
+        <v>7</v>
+      </c>
       <c r="E11" s="59"/>
       <c r="F11" s="54"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
+      <c r="G11" s="50">
+        <v>7</v>
+      </c>
+      <c r="H11" s="44">
+        <v>7</v>
+      </c>
+      <c r="I11" s="44">
+        <v>7</v>
+      </c>
+      <c r="J11" s="50">
+        <v>7</v>
+      </c>
+      <c r="K11" s="50">
+        <v>7</v>
+      </c>
       <c r="L11" s="54"/>
       <c r="M11" s="54"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="50"/>
+      <c r="N11" s="50">
+        <v>7</v>
+      </c>
+      <c r="O11" s="50">
+        <v>7</v>
+      </c>
+      <c r="P11" s="50">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="50">
+        <v>7</v>
+      </c>
+      <c r="R11" s="50">
+        <v>7</v>
+      </c>
       <c r="S11" s="54"/>
       <c r="T11" s="54"/>
       <c r="U11" s="50"/>
@@ -1736,7 +1763,7 @@
       <c r="AF11" s="50"/>
       <c r="AG11" s="44">
         <f>SUM(C11:AF11)</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="AH11" s="62"/>
       <c r="AI11" s="64"/>
@@ -1744,7 +1771,7 @@
     <row r="12" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A12" s="36"/>
       <c r="B12" s="47" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
@@ -1764,11 +1791,21 @@
       <c r="R12" s="50"/>
       <c r="S12" s="54"/>
       <c r="T12" s="54"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="50"/>
+      <c r="U12" s="50">
+        <v>7</v>
+      </c>
+      <c r="V12" s="50">
+        <v>7</v>
+      </c>
+      <c r="W12" s="50">
+        <v>7</v>
+      </c>
+      <c r="X12" s="50">
+        <v>7</v>
+      </c>
+      <c r="Y12" s="50">
+        <v>7</v>
+      </c>
       <c r="Z12" s="54"/>
       <c r="AA12" s="54"/>
       <c r="AB12" s="50"/>
@@ -1778,7 +1815,7 @@
       <c r="AF12" s="50"/>
       <c r="AG12" s="44">
         <f>SUM(C12:AF12)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="AH12" s="62"/>
       <c r="AI12" s="64"/>
@@ -1786,11 +1823,11 @@
     <row r="13" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A13" s="36"/>
       <c r="B13" s="47" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
-      <c r="E13" s="59"/>
+      <c r="E13" s="60"/>
       <c r="F13" s="54"/>
       <c r="G13" s="50"/>
       <c r="H13" s="44"/>
@@ -1813,204 +1850,266 @@
       <c r="Y13" s="50"/>
       <c r="Z13" s="54"/>
       <c r="AA13" s="54"/>
-      <c r="AB13" s="50"/>
-      <c r="AC13" s="50"/>
-      <c r="AD13" s="50"/>
-      <c r="AE13" s="50"/>
-      <c r="AF13" s="50"/>
+      <c r="AB13" s="50">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="50">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="50">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="50">
+        <v>3</v>
+      </c>
+      <c r="AF13" s="50">
+        <v>3</v>
+      </c>
       <c r="AG13" s="44">
-        <f>SUM(C13:AF13)</f>
-        <v>0</v>
+        <f t="shared" ref="AG13:AG14" si="0">SUM(C13:AF13)</f>
+        <v>15</v>
       </c>
       <c r="AH13" s="62"/>
       <c r="AI13" s="64"/>
     </row>
-    <row r="14" spans="1:146" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
+      <c r="A14" s="36"/>
+      <c r="B14" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="54"/>
+      <c r="AA14" s="54"/>
+      <c r="AB14" s="50">
+        <v>4</v>
+      </c>
+      <c r="AC14" s="50">
+        <v>4</v>
+      </c>
+      <c r="AD14" s="50">
+        <v>4</v>
+      </c>
+      <c r="AE14" s="50">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="50">
+        <v>4</v>
+      </c>
+      <c r="AG14" s="44">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AH14" s="62"/>
+      <c r="AI14" s="64"/>
+    </row>
+    <row r="15" spans="1:146" s="4" customFormat="1" ht="36" customHeight="1">
+      <c r="A15" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="51">
-        <f t="shared" ref="C14:AF14" si="0">SUM(C10:C13)</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="55">
-        <f t="shared" si="0"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="51">
+        <f t="shared" ref="C15:AF15" si="1">SUM(C10:C14)</f>
+        <v>8</v>
+      </c>
+      <c r="D15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="55">
-        <f t="shared" si="0"/>
+      <c r="F15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H14" s="45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L14" s="55">
-        <f t="shared" si="0"/>
+      <c r="G15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H15" s="45">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I15" s="45">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M14" s="55">
-        <f t="shared" si="0"/>
+      <c r="M15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S14" s="55">
-        <f t="shared" si="0"/>
+      <c r="N15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="O15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="P15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="R15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="S15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T14" s="55">
-        <f t="shared" si="0"/>
+      <c r="T15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="W14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="X14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Y14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Z14" s="55">
-        <f t="shared" si="0"/>
+      <c r="U15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="V15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="W15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="X15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Y15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Z15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="55">
-        <f t="shared" si="0"/>
+      <c r="AA15" s="55">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AC14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AD14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AE14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AF14" s="51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AG14" s="45">
-        <f>SUM(C14:AF14)</f>
-        <v>22</v>
-      </c>
-      <c r="AH14" s="39"/>
-      <c r="AI14" s="40"/>
+      <c r="AB15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AC15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AD15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AE15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AF15" s="51">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AG15" s="45">
+        <f>SUM(C15:AF15)</f>
+        <v>176</v>
+      </c>
+      <c r="AH15" s="39"/>
+      <c r="AI15" s="40"/>
     </row>
-    <row r="15" spans="1:146" ht="23.25" customHeight="1">
-      <c r="A15" s="41" t="s">
+    <row r="16" spans="1:146" ht="23.25" customHeight="1">
+      <c r="A16" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="42"/>
     </row>
-    <row r="16" spans="1:146" ht="14.5">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+    <row r="17" spans="1:26" ht="14.5">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
     </row>
-    <row r="17" spans="26:26">
-      <c r="Z17" s="21"/>
+    <row r="18" spans="1:26">
+      <c r="Z18" s="21"/>
     </row>
-    <row r="18" spans="26:26">
-      <c r="Z18" s="22"/>
+    <row r="19" spans="1:26">
+      <c r="Z19" s="22"/>
     </row>
-    <row r="19" spans="26:26" ht="12.75" customHeight="1">
-      <c r="Z19" s="22"/>
+    <row r="20" spans="1:26" ht="12.75" customHeight="1">
+      <c r="Z20" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="AH10:AH13"/>
-    <mergeCell ref="AI10:AI13"/>
+    <mergeCell ref="AH10:AH14"/>
+    <mergeCell ref="AI10:AI14"/>
     <mergeCell ref="C6:N6"/>
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="S5:T5"/>
@@ -2020,7 +2119,7 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.19" header="0.5" footer="0.16"/>
-  <pageSetup paperSize="9" scale="31" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="33" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>